<commit_message>
Add flow optimised value stream
</commit_message>
<xml_diff>
--- a/data/ExampleValueStream.xlsx
+++ b/data/ExampleValueStream.xlsx
@@ -5,10 +5,11 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="0"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="988" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Value Stream" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Resource Optimised" sheetId="1" state="visible" r:id="rId2"/>
+    <sheet name="Flow Optimised" sheetId="2" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr iterateCount="1" refMode="A1" iterate="false" iterateDelta="0.0001"/>
   <extLst>
@@ -20,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="119" uniqueCount="65">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="162" uniqueCount="80">
   <si>
     <t xml:space="preserve">Days</t>
   </si>
@@ -215,6 +216,51 @@
   </si>
   <si>
     <t xml:space="preserve">Application release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Create story ticket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Research and analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Draft specification</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait for specification workshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification workshop</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Specification linked to story</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PO authorises story ticket</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Automate specification checks</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Code and automated tests</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait for build pipeline</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait for QA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Exploratory testing</t>
+  </si>
+  <si>
+    <t xml:space="preserve">QA sign off</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Wait for application release</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Close story ticket</t>
   </si>
 </sst>
 </file>
@@ -267,7 +313,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right/>
@@ -304,13 +350,6 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top/>
-      <bottom style="thin"/>
-      <diagonal/>
-    </border>
-    <border diagonalUp="false" diagonalDown="false">
       <left/>
       <right style="thin"/>
       <top/>
@@ -325,17 +364,17 @@
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
+      <left/>
       <right style="thin"/>
       <top style="thin"/>
       <bottom/>
       <diagonal/>
     </border>
     <border diagonalUp="false" diagonalDown="false">
-      <left/>
+      <left style="thin"/>
       <right style="thin"/>
-      <top style="thin"/>
-      <bottom/>
+      <top/>
+      <bottom style="thin"/>
       <diagonal/>
     </border>
   </borders>
@@ -403,19 +442,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="true" applyBorder="true" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="166" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -423,15 +470,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="9" xfId="0" applyFont="false" applyBorder="true" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="19" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -444,6 +483,32 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
     <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
+  <dxfs count="3">
+    <dxf>
+      <font>
+        <name val="Frutiger 45 Light"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Frutiger 45 Light"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <name val="Frutiger 45 Light"/>
+        <charset val="1"/>
+        <family val="2"/>
+        <color rgb="FF000000"/>
+      </font>
+    </dxf>
+  </dxfs>
 </styleSheet>
 </file>
 
@@ -469,17 +534,17 @@
   </sheetPr>
   <dimension ref="B1:H62"/>
   <sheetViews>
-    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A12" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D35" activeCellId="0" sqref="D35"/>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H62" activeCellId="0" sqref="H62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8"/>
   <cols>
-    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="11.936170212766"/>
-    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="33.4382978723404"/>
-    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="13.9617021276596"/>
-    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="9.34468085106383"/>
-    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="7.54468085106383"/>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0723404255319"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.6297872340426"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5489361702128"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9191489361702"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.8936170212766"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -505,7 +570,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B2" s="2" t="n">
         <f aca="false">C2/8</f>
         <v>0</v>
@@ -530,7 +595,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B3" s="2" t="n">
         <f aca="false">C3/8</f>
         <v>0.0125</v>
@@ -556,7 +621,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B4" s="2" t="n">
         <f aca="false">C4/8</f>
         <v>2.0125</v>
@@ -582,7 +647,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B5" s="2" t="n">
         <f aca="false">C5/8</f>
         <v>4.0125</v>
@@ -608,7 +673,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B6" s="2" t="n">
         <f aca="false">C6/8</f>
         <v>4.1375</v>
@@ -634,7 +699,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B7" s="2" t="n">
         <f aca="false">C7/8</f>
         <v>4.15</v>
@@ -660,7 +725,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B8" s="2" t="n">
         <f aca="false">C8/8</f>
         <v>4.1625</v>
@@ -686,7 +751,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B9" s="2" t="n">
         <f aca="false">C9/8</f>
         <v>6.6625</v>
@@ -712,7 +777,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B10" s="2" t="n">
         <f aca="false">C10/8</f>
         <v>7.1625</v>
@@ -738,7 +803,7 @@
         <v>1.875</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B11" s="2" t="n">
         <f aca="false">C11/8</f>
         <v>7.175</v>
@@ -764,7 +829,7 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B12" s="2" t="n">
         <f aca="false">C12/8</f>
         <v>7.2125</v>
@@ -790,7 +855,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B13" s="2" t="n">
         <f aca="false">C13/8</f>
         <v>7.3375</v>
@@ -816,7 +881,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B14" s="2" t="n">
         <f aca="false">C14/8</f>
         <v>9.3375</v>
@@ -842,7 +907,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B15" s="2" t="n">
         <f aca="false">C15/8</f>
         <v>9.4625</v>
@@ -868,7 +933,7 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="2" t="n">
         <f aca="false">C16/8</f>
         <v>9.8375</v>
@@ -880,13 +945,13 @@
       <c r="D16" s="8" t="s">
         <v>24</v>
       </c>
-      <c r="E16" s="9" t="s">
+      <c r="E16" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F16" s="10" t="n">
+      <c r="F16" s="9" t="n">
         <v>20</v>
       </c>
-      <c r="G16" s="11" t="n">
+      <c r="G16" s="10" t="n">
         <v>1.7</v>
       </c>
       <c r="H16" s="7" t="n">
@@ -894,7 +959,7 @@
         <v>31.875</v>
       </c>
     </row>
-    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="17" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B17" s="2" t="n">
         <f aca="false">C17/8</f>
         <v>10.05</v>
@@ -920,7 +985,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="18" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B18" s="2" t="n">
         <f aca="false">C18/8</f>
         <v>15.05</v>
@@ -929,16 +994,16 @@
         <f aca="false">C17+G17</f>
         <v>120.4</v>
       </c>
-      <c r="D18" s="12" t="s">
+      <c r="D18" s="11" t="s">
         <v>26</v>
       </c>
-      <c r="E18" s="13" t="s">
-        <v>8</v>
-      </c>
-      <c r="F18" s="14" t="n">
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="12" t="n">
         <v>5</v>
       </c>
-      <c r="G18" s="15" t="n">
+      <c r="G18" s="13" t="n">
         <v>1</v>
       </c>
       <c r="H18" s="7" t="n">
@@ -946,7 +1011,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="19" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="19" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B19" s="2" t="n">
         <f aca="false">C19/8</f>
         <v>15.175</v>
@@ -972,7 +1037,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="20" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="20" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B20" s="2" t="n">
         <f aca="false">C20/8</f>
         <v>15.3</v>
@@ -998,7 +1063,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="21" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="21" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B21" s="2" t="n">
         <f aca="false">C21/8</f>
         <v>15.425</v>
@@ -1024,7 +1089,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="22" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="22" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B22" s="2" t="n">
         <f aca="false">C22/8</f>
         <v>15.4875</v>
@@ -1050,7 +1115,7 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="23" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="23" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B23" s="2" t="n">
         <f aca="false">C23/8</f>
         <v>15.525</v>
@@ -1076,7 +1141,7 @@
         <v>375</v>
       </c>
     </row>
-    <row r="24" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="24" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B24" s="2" t="n">
         <f aca="false">C24/8</f>
         <v>18.025</v>
@@ -1102,7 +1167,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="25" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="25" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B25" s="2" t="n">
         <f aca="false">C25/8</f>
         <v>18.15</v>
@@ -1128,7 +1193,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="26" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="26" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B26" s="2" t="n">
         <f aca="false">C26/8</f>
         <v>19.15</v>
@@ -1154,7 +1219,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="27" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="27" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B27" s="2" t="n">
         <f aca="false">C27/8</f>
         <v>20.15</v>
@@ -1180,7 +1245,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="28" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="28" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B28" s="2" t="n">
         <f aca="false">C28/8</f>
         <v>21.15</v>
@@ -1206,7 +1271,7 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="29" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="29" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B29" s="2" t="n">
         <f aca="false">C29/8</f>
         <v>21.1875</v>
@@ -1232,7 +1297,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="30" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="30" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B30" s="2" t="n">
         <f aca="false">C30/8</f>
         <v>21.4375</v>
@@ -1258,7 +1323,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="31" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="31" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B31" s="2" t="n">
         <f aca="false">C31/8</f>
         <v>21.4625</v>
@@ -1284,7 +1349,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="32" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="32" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B32" s="2" t="n">
         <f aca="false">C32/8</f>
         <v>21.7125</v>
@@ -1310,7 +1375,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="33" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="33" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B33" s="2" t="n">
         <f aca="false">C33/8</f>
         <v>21.775</v>
@@ -1334,7 +1399,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="34" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="34" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B34" s="2" t="n">
         <f aca="false">C34/8</f>
         <v>22.275</v>
@@ -1360,7 +1425,7 @@
         <v>93.75</v>
       </c>
     </row>
-    <row r="35" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="35" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B35" s="2" t="n">
         <f aca="false">C35/8</f>
         <v>22.9</v>
@@ -1386,7 +1451,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="36" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="36" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B36" s="2" t="n">
         <f aca="false">C36/8</f>
         <v>22.925</v>
@@ -1412,7 +1477,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="37" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="37" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B37" s="2" t="n">
         <f aca="false">C37/8</f>
         <v>23.425</v>
@@ -1438,7 +1503,7 @@
         <v>750</v>
       </c>
     </row>
-    <row r="38" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="38" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B38" s="2" t="n">
         <f aca="false">C38/8</f>
         <v>28.425</v>
@@ -1464,7 +1529,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="39" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="39" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B39" s="2" t="n">
         <f aca="false">C39/8</f>
         <v>28.55</v>
@@ -1473,16 +1538,16 @@
         <f aca="false">C38+G38</f>
         <v>228.4</v>
       </c>
-      <c r="D39" s="12" t="s">
+      <c r="D39" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="F39" s="14" t="n">
+      <c r="F39" s="12" t="n">
         <v>0</v>
       </c>
-      <c r="G39" s="15" t="n">
+      <c r="G39" s="13" t="n">
         <v>80</v>
       </c>
       <c r="H39" s="7" t="n">
@@ -1490,7 +1555,7 @@
         <v>1500</v>
       </c>
     </row>
-    <row r="40" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="40" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B40" s="2" t="n">
         <f aca="false">C40/8</f>
         <v>38.55</v>
@@ -1516,7 +1581,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="41" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B41" s="2" t="n">
         <f aca="false">C41/8</f>
         <v>38.575</v>
@@ -1542,7 +1607,7 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="42" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B42" s="2" t="n">
         <f aca="false">C42/8</f>
         <v>38.825</v>
@@ -1568,7 +1633,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="43" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B43" s="2" t="n">
         <f aca="false">C43/8</f>
         <v>39.825</v>
@@ -1594,7 +1659,7 @@
         <v>56.25</v>
       </c>
     </row>
-    <row r="44" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="44" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B44" s="2" t="n">
         <f aca="false">C44/8</f>
         <v>40.2</v>
@@ -1620,7 +1685,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="45" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="45" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B45" s="2" t="n">
         <f aca="false">C45/8</f>
         <v>40.225</v>
@@ -1646,7 +1711,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="46" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="46" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B46" s="2" t="n">
         <f aca="false">C46/8</f>
         <v>40.35</v>
@@ -1672,7 +1737,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="47" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="47" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B47" s="2" t="n">
         <f aca="false">C47/8</f>
         <v>40.85</v>
@@ -1698,7 +1763,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="48" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="48" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B48" s="2" t="n">
         <f aca="false">C48/8</f>
         <v>40.875</v>
@@ -1724,7 +1789,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="49" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="49" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B49" s="2" t="n">
         <f aca="false">C49/8</f>
         <v>41.875</v>
@@ -1750,7 +1815,7 @@
         <v>3.75</v>
       </c>
     </row>
-    <row r="50" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="50" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B50" s="2" t="n">
         <f aca="false">C50/8</f>
         <v>41.9</v>
@@ -1776,7 +1841,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="51" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="51" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B51" s="2" t="n">
         <f aca="false">C51/8</f>
         <v>41.9625</v>
@@ -1802,7 +1867,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="52" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="52" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B52" s="2" t="n">
         <f aca="false">C52/8</f>
         <v>42.025</v>
@@ -1828,7 +1893,7 @@
         <v>9.375</v>
       </c>
     </row>
-    <row r="53" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="53" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B53" s="2" t="n">
         <f aca="false">C53/8</f>
         <v>42.0875</v>
@@ -1854,7 +1919,7 @@
         <v>18.75</v>
       </c>
     </row>
-    <row r="54" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="54" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B54" s="2" t="n">
         <f aca="false">C54/8</f>
         <v>42.2125</v>
@@ -1880,7 +1945,7 @@
         <v>5.625</v>
       </c>
     </row>
-    <row r="55" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="55" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B55" s="2" t="n">
         <f aca="false">C55/8</f>
         <v>42.25</v>
@@ -1906,7 +1971,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="56" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="56" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B56" s="2" t="n">
         <f aca="false">C56/8</f>
         <v>44.25</v>
@@ -1932,8 +1997,11 @@
         <v>37.5</v>
       </c>
     </row>
-    <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
-    <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="57" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E57" s="4"/>
+    </row>
+    <row r="58" customFormat="false" ht="13.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E58" s="4"/>
       <c r="G58" s="2" t="n">
         <f aca="false">SUM(G2:G56)</f>
         <v>356</v>
@@ -1943,8 +2011,8 @@
         <v>44.5</v>
       </c>
     </row>
-    <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E59" s="0" t="s">
+    <row r="59" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E59" s="4" t="s">
         <v>10</v>
       </c>
       <c r="G59" s="0" t="n">
@@ -1956,8 +2024,8 @@
         <v>6.8</v>
       </c>
     </row>
-    <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="E60" s="0" t="s">
+    <row r="60" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E60" s="4" t="s">
         <v>8</v>
       </c>
       <c r="G60" s="0" t="n">
@@ -1971,12 +2039,661 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="H62" s="16" t="n">
+      <c r="H62" s="14" t="n">
         <f aca="false">H59/H58</f>
         <v>0.152808988764045</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="E2">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E3">
+    <cfRule type="cellIs" priority="5" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="6" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="7" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E4">
+    <cfRule type="cellIs" priority="8" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="9" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="10" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E5">
+    <cfRule type="cellIs" priority="11" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="12" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="13" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E6">
+    <cfRule type="cellIs" priority="14" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="15" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="16" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E7">
+    <cfRule type="cellIs" priority="17" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="18" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="19" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E8">
+    <cfRule type="cellIs" priority="20" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="21" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="22" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E9">
+    <cfRule type="cellIs" priority="23" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="24" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="25" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E10">
+    <cfRule type="cellIs" priority="26" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="27" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="28" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E11">
+    <cfRule type="cellIs" priority="29" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="30" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="31" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E12">
+    <cfRule type="cellIs" priority="32" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="33" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="34" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E13">
+    <cfRule type="cellIs" priority="35" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="36" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="37" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E14">
+    <cfRule type="cellIs" priority="38" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="39" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="40" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E15">
+    <cfRule type="cellIs" priority="41" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="42" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="43" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E16">
+    <cfRule type="cellIs" priority="44" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="45" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="46" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E17">
+    <cfRule type="cellIs" priority="47" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="48" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="49" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" priority="50" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="51" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="52" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E19">
+    <cfRule type="cellIs" priority="53" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="54" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="55" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E20">
+    <cfRule type="cellIs" priority="56" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="57" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="58" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E21">
+    <cfRule type="cellIs" priority="59" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="60" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="61" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E22">
+    <cfRule type="cellIs" priority="62" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="63" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="64" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E23">
+    <cfRule type="cellIs" priority="65" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="66" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="67" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E24">
+    <cfRule type="cellIs" priority="68" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="69" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="70" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E25">
+    <cfRule type="cellIs" priority="71" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="72" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="73" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E26">
+    <cfRule type="cellIs" priority="74" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="75" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="76" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E27">
+    <cfRule type="cellIs" priority="77" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="78" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="79" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E28">
+    <cfRule type="cellIs" priority="80" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="81" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="82" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E29">
+    <cfRule type="cellIs" priority="83" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="84" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="85" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E30">
+    <cfRule type="cellIs" priority="86" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="87" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="88" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E31">
+    <cfRule type="cellIs" priority="89" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="90" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="91" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E32">
+    <cfRule type="cellIs" priority="92" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="93" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="94" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E33">
+    <cfRule type="cellIs" priority="95" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="96" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="97" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E34">
+    <cfRule type="cellIs" priority="98" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="99" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="100" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E35">
+    <cfRule type="cellIs" priority="101" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="102" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="103" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E36">
+    <cfRule type="cellIs" priority="104" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="105" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="106" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E37">
+    <cfRule type="cellIs" priority="107" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="108" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="109" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E38">
+    <cfRule type="cellIs" priority="110" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="111" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="112" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E39">
+    <cfRule type="cellIs" priority="113" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="114" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="115" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E40">
+    <cfRule type="cellIs" priority="116" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="117" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="118" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E41">
+    <cfRule type="cellIs" priority="119" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="120" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="121" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E42">
+    <cfRule type="cellIs" priority="122" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="123" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="124" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E43">
+    <cfRule type="cellIs" priority="125" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="126" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="127" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E44">
+    <cfRule type="cellIs" priority="128" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="129" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="130" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E45">
+    <cfRule type="cellIs" priority="131" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="132" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="133" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E46">
+    <cfRule type="cellIs" priority="134" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="135" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="136" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E47">
+    <cfRule type="cellIs" priority="137" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="138" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="139" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E48">
+    <cfRule type="cellIs" priority="140" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="141" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="142" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E49">
+    <cfRule type="cellIs" priority="143" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="144" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="145" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E50">
+    <cfRule type="cellIs" priority="146" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="147" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="148" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E51">
+    <cfRule type="cellIs" priority="149" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="150" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="151" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E52">
+    <cfRule type="cellIs" priority="152" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="153" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="154" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E53">
+    <cfRule type="cellIs" priority="155" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="156" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="157" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E54">
+    <cfRule type="cellIs" priority="158" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="159" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="160" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E55">
+    <cfRule type="cellIs" priority="161" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="162" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="163" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E56">
+    <cfRule type="cellIs" priority="164" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="165" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="166" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E57">
+    <cfRule type="cellIs" priority="167" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="168" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="169" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E58">
+    <cfRule type="cellIs" priority="170" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="171" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="172" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E59">
+    <cfRule type="cellIs" priority="173" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="174" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="175" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="E60">
+    <cfRule type="cellIs" priority="176" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="177" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="178" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
   <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -1988,4 +2705,554 @@
     <tablePart r:id="rId1"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="B1:H24"/>
+  <sheetViews>
+    <sheetView windowProtection="false" showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E2" activeCellId="0" sqref="E2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.8"/>
+  <cols>
+    <col collapsed="false" hidden="false" max="3" min="3" style="0" width="14.0723404255319"/>
+    <col collapsed="false" hidden="false" max="4" min="4" style="0" width="39.6297872340426"/>
+    <col collapsed="false" hidden="false" max="5" min="5" style="0" width="16.5489361702128"/>
+    <col collapsed="false" hidden="false" max="6" min="6" style="0" width="10.9191489361702"/>
+    <col collapsed="false" hidden="false" max="7" min="7" style="0" width="8.8936170212766"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B2" s="2" t="n">
+        <f aca="false">C2/8</f>
+        <v>0</v>
+      </c>
+      <c r="C2" s="2" t="n">
+        <v>0</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="E2" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F2" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G2" s="6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H2" s="7" t="n">
+        <f aca="false">G2*18.75</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B3" s="2" t="n">
+        <f aca="false">C3/8</f>
+        <v>0.0125</v>
+      </c>
+      <c r="C3" s="2" t="n">
+        <f aca="false">C2+G2</f>
+        <v>0.1</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G3" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H3" s="7" t="n">
+        <f aca="false">G3*18.75</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B4" s="2" t="n">
+        <f aca="false">C4/8</f>
+        <v>0.5125</v>
+      </c>
+      <c r="C4" s="2" t="n">
+        <f aca="false">C3+G3</f>
+        <v>4.1</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>67</v>
+      </c>
+      <c r="E4" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F4" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G4" s="6" t="n">
+        <v>2</v>
+      </c>
+      <c r="H4" s="7" t="n">
+        <f aca="false">G4*18.75</f>
+        <v>37.5</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B5" s="2" t="n">
+        <f aca="false">C5/8</f>
+        <v>0.7625</v>
+      </c>
+      <c r="C5" s="2" t="n">
+        <f aca="false">C4+G4</f>
+        <v>6.1</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="E5" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G5" s="6" t="n">
+        <v>4</v>
+      </c>
+      <c r="H5" s="7" t="n">
+        <f aca="false">G5*18.75</f>
+        <v>75</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B6" s="2" t="n">
+        <f aca="false">C6/8</f>
+        <v>1.2625</v>
+      </c>
+      <c r="C6" s="2" t="n">
+        <f aca="false">C5+G5</f>
+        <v>10.1</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="E6" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F6" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G6" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H6" s="7" t="n">
+        <f aca="false">G6*18.75</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B7" s="2" t="n">
+        <f aca="false">C7/8</f>
+        <v>1.3875</v>
+      </c>
+      <c r="C7" s="2" t="n">
+        <f aca="false">C6+G6</f>
+        <v>11.1</v>
+      </c>
+      <c r="D7" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="E7" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F7" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G7" s="6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H7" s="7" t="n">
+        <f aca="false">G7*18.75</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B8" s="2" t="n">
+        <f aca="false">C8/8</f>
+        <v>1.4</v>
+      </c>
+      <c r="C8" s="2" t="n">
+        <f aca="false">C7+G7</f>
+        <v>11.2</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="E8" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F8" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G8" s="6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H8" s="7" t="n">
+        <f aca="false">G8*18.75</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B9" s="2" t="n">
+        <f aca="false">C9/8</f>
+        <v>1.4125</v>
+      </c>
+      <c r="C9" s="2" t="n">
+        <f aca="false">C8+G8</f>
+        <v>11.3</v>
+      </c>
+      <c r="D9" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="E9" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F9" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G9" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="H9" s="7" t="n">
+        <f aca="false">G9*18.75</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B10" s="2" t="n">
+        <f aca="false">C10/8</f>
+        <v>2.4125</v>
+      </c>
+      <c r="C10" s="2" t="n">
+        <f aca="false">C9+G9</f>
+        <v>19.3</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>72</v>
+      </c>
+      <c r="E10" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F10" s="5" t="n">
+        <v>2</v>
+      </c>
+      <c r="G10" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="H10" s="7" t="n">
+        <f aca="false">G10*18.75</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B11" s="2" t="n">
+        <f aca="false">C11/8</f>
+        <v>3.4125</v>
+      </c>
+      <c r="C11" s="2" t="n">
+        <f aca="false">C10+G10</f>
+        <v>27.3</v>
+      </c>
+      <c r="D11" s="3" t="s">
+        <v>73</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F11" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="G11" s="6" t="n">
+        <v>8</v>
+      </c>
+      <c r="H11" s="7" t="n">
+        <f aca="false">G11*18.75</f>
+        <v>150</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B12" s="2" t="n">
+        <f aca="false">C12/8</f>
+        <v>4.4125</v>
+      </c>
+      <c r="C12" s="2" t="n">
+        <f aca="false">C11+G11</f>
+        <v>35.3</v>
+      </c>
+      <c r="D12" s="3" t="s">
+        <v>74</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G12" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H12" s="7" t="n">
+        <f aca="false">G12*18.75</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B13" s="2" t="n">
+        <f aca="false">C13/8</f>
+        <v>4.5375</v>
+      </c>
+      <c r="C13" s="2" t="n">
+        <f aca="false">C12+G12</f>
+        <v>36.3</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>75</v>
+      </c>
+      <c r="E13" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F13" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G13" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H13" s="7" t="n">
+        <f aca="false">G13*18.75</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="13.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B14" s="2" t="n">
+        <f aca="false">C14/8</f>
+        <v>4.6625</v>
+      </c>
+      <c r="C14" s="2" t="n">
+        <f aca="false">C13+G13</f>
+        <v>37.3</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="E14" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="F14" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G14" s="6" t="n">
+        <v>1</v>
+      </c>
+      <c r="H14" s="7" t="n">
+        <f aca="false">G14*18.75</f>
+        <v>18.75</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B15" s="2" t="n">
+        <f aca="false">C15/8</f>
+        <v>4.7875</v>
+      </c>
+      <c r="C15" s="2" t="n">
+        <f aca="false">C14+G14</f>
+        <v>38.3</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="E15" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F15" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G15" s="6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H15" s="7" t="n">
+        <f aca="false">G15*18.75</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B16" s="2" t="n">
+        <f aca="false">C16/8</f>
+        <v>4.8</v>
+      </c>
+      <c r="C16" s="2" t="n">
+        <f aca="false">C15+G15</f>
+        <v>38.4</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="E16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="5" t="n">
+        <v>0</v>
+      </c>
+      <c r="G16" s="6" t="n">
+        <v>1.4</v>
+      </c>
+      <c r="H16" s="7" t="n">
+        <f aca="false">G16*18.75</f>
+        <v>26.25</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B17" s="2" t="n">
+        <f aca="false">C17/8</f>
+        <v>4.975</v>
+      </c>
+      <c r="C17" s="2" t="n">
+        <f aca="false">C16+G16</f>
+        <v>39.8</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>64</v>
+      </c>
+      <c r="E17" s="15" t="s">
+        <v>10</v>
+      </c>
+      <c r="F17" s="9" t="n">
+        <v>1</v>
+      </c>
+      <c r="G17" s="10" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H17" s="7" t="n">
+        <f aca="false">G17*18.75</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="13.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B18" s="2" t="n">
+        <f aca="false">C18/8</f>
+        <v>4.9875</v>
+      </c>
+      <c r="C18" s="2" t="n">
+        <f aca="false">C17+G17</f>
+        <v>39.9</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E18" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="F18" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="G18" s="6" t="n">
+        <v>0.1</v>
+      </c>
+      <c r="H18" s="7" t="n">
+        <f aca="false">G18*18.75</f>
+        <v>1.875</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="G20" s="2" t="n">
+        <f aca="false">SUM(G2:G18)</f>
+        <v>40</v>
+      </c>
+      <c r="H20" s="7" t="n">
+        <f aca="false">G20/8</f>
+        <v>5</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E21" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G21" s="0" t="n">
+        <f aca="false">SUMIF($E$2:$E$18,E21,$G$2:$G$18)</f>
+        <v>32.1</v>
+      </c>
+      <c r="H21" s="7" t="n">
+        <f aca="false">G21/8</f>
+        <v>4.0125</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="E22" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="G22" s="0" t="n">
+        <f aca="false">SUMIF($E$2:$E$18,E22,$G$2:$G$18)</f>
+        <v>0.5</v>
+      </c>
+      <c r="H22" s="7" t="n">
+        <f aca="false">G22/8</f>
+        <v>0.0625</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="14" t="n">
+        <f aca="false">H21/H20</f>
+        <v>0.8025</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="E18">
+    <cfRule type="cellIs" priority="2" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="0">
+      <formula>"Required waste"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="3" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="1">
+      <formula>"Value add"</formula>
+    </cfRule>
+    <cfRule type="cellIs" priority="4" operator="equal" aboveAverage="0" equalAverage="0" bottom="0" percent="0" rank="0" text="" dxfId="2">
+      <formula>"Queue"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511805555555555" footer="0.511805555555555"/>
+  <pageSetup paperSize="9" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" usePrinterDefaults="false" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader/>
+    <oddFooter/>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>